<commit_message>
Add [API Design] Post module docs
</commit_message>
<xml_diff>
--- a/doc/backend/api/TRN-MiniBlog_API_User_Change_Password_DetailedDesign-TuanNguyen.xlsx
+++ b/doc/backend/api/TRN-MiniBlog_API_User_Change_Password_DetailedDesign-TuanNguyen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7890" tabRatio="898"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="20490" windowHeight="7890" tabRatio="898" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="101">
   <si>
     <t>Overview</t>
   </si>
@@ -272,13 +272,7 @@
     <t>A</t>
   </si>
   <si>
-    <t>nguyen.kiet</t>
-  </si>
-  <si>
     <t>MiniBlog</t>
-  </si>
-  <si>
-    <t>2015/02/10</t>
   </si>
   <si>
     <t>Input data validate</t>
@@ -338,9 +332,6 @@
     <t>09/10/2015</t>
   </si>
   <si>
-    <t>2004</t>
-  </si>
-  <si>
     <t>The token field is invalid.</t>
   </si>
   <si>
@@ -366,6 +357,9 @@
   </si>
   <si>
     <t>/*bcrypt('password'), 1*/</t>
+  </si>
+  <si>
+    <t>1504</t>
   </si>
 </sst>
 </file>
@@ -1376,6 +1370,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="6" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1402,27 +1417,6 @@
     </xf>
     <xf numFmtId="49" fontId="12" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="117">
@@ -2776,7 +2770,7 @@
               </a:effectLst>
               <a:latin typeface="+mn-lt"/>
             </a:rPr>
-            <a:t>Set code = 2004</a:t>
+            <a:t>Set code = 1504</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3595,7 +3589,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>27354</xdr:colOff>
+      <xdr:colOff>27353</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>14680</xdr:rowOff>
     </xdr:to>
@@ -3621,7 +3615,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1709367" y="4482385"/>
-          <a:ext cx="6919062" cy="5962170"/>
+          <a:ext cx="6919061" cy="5962170"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4957,7 +4951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B26" sqref="B26:H26"/>
     </sheetView>
@@ -4989,14 +4983,14 @@
       </c>
       <c r="C4" s="117"/>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="116" t="s">
         <v>23</v>
       </c>
       <c r="F4" s="117"/>
       <c r="G4" s="114" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" s="115"/>
     </row>
@@ -5021,7 +5015,7 @@
       </c>
       <c r="C6" s="117"/>
       <c r="D6" s="120" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E6" s="116" t="s">
         <v>30</v>
@@ -5131,7 +5125,7 @@
         <v>69</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E11" s="56" t="s">
         <v>70</v>
@@ -5140,10 +5134,10 @@
         <v>42286</v>
       </c>
       <c r="G11" s="53" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" s="55" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I11" s="46"/>
       <c r="J11" s="46"/>
@@ -5624,7 +5618,7 @@
   <dimension ref="B1:BM23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AY5" sqref="AY5"/>
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -5705,7 +5699,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -5721,7 +5715,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -5998,7 +5992,7 @@
       <c r="AP8" s="89"/>
       <c r="AQ8" s="90"/>
       <c r="AR8" s="88" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AS8" s="89"/>
       <c r="AT8" s="89"/>
@@ -6022,7 +6016,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="81"/>
       <c r="E9" s="81"/>
@@ -6033,7 +6027,7 @@
       <c r="J9" s="81"/>
       <c r="K9" s="82"/>
       <c r="L9" s="81" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M9" s="81"/>
       <c r="N9" s="81"/>
@@ -6055,14 +6049,14 @@
       <c r="AD9" s="81"/>
       <c r="AE9" s="82"/>
       <c r="AF9" s="80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AG9" s="81"/>
       <c r="AH9" s="81"/>
       <c r="AI9" s="81"/>
       <c r="AJ9" s="82"/>
       <c r="AK9" s="80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AL9" s="81"/>
       <c r="AM9" s="81"/>
@@ -6071,7 +6065,7 @@
       <c r="AP9" s="81"/>
       <c r="AQ9" s="82"/>
       <c r="AR9" s="80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AS9" s="81"/>
       <c r="AT9" s="81"/>
@@ -6080,7 +6074,7 @@
       <c r="AW9" s="81"/>
       <c r="AX9" s="81"/>
       <c r="AY9" s="83" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AZ9" s="84"/>
       <c r="BA9" s="84"/>
@@ -6092,10 +6086,10 @@
     </row>
     <row r="10" spans="2:65" ht="15.75" customHeight="1">
       <c r="B10" s="86" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
@@ -6106,7 +6100,7 @@
       <c r="J10" s="81"/>
       <c r="K10" s="82"/>
       <c r="L10" s="81" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M10" s="81"/>
       <c r="N10" s="81"/>
@@ -6128,14 +6122,14 @@
       <c r="AD10" s="81"/>
       <c r="AE10" s="82"/>
       <c r="AF10" s="80" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="AG10" s="81"/>
       <c r="AH10" s="81"/>
       <c r="AI10" s="81"/>
       <c r="AJ10" s="82"/>
       <c r="AK10" s="80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AL10" s="81"/>
       <c r="AM10" s="81"/>
@@ -6144,7 +6138,7 @@
       <c r="AP10" s="81"/>
       <c r="AQ10" s="82"/>
       <c r="AR10" s="80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AS10" s="81"/>
       <c r="AT10" s="81"/>
@@ -6153,7 +6147,7 @@
       <c r="AW10" s="81"/>
       <c r="AX10" s="81"/>
       <c r="AY10" s="83" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="AZ10" s="84"/>
       <c r="BA10" s="84"/>
@@ -7013,7 +7007,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -7029,7 +7023,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -7340,7 +7334,7 @@
       <c r="B9" s="99"/>
       <c r="C9" s="100"/>
       <c r="D9" s="101" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="96"/>
       <c r="F9" s="96"/>
@@ -7480,7 +7474,7 @@
       <c r="D11" s="95"/>
       <c r="E11" s="95"/>
       <c r="F11" s="95" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
@@ -7550,7 +7544,7 @@
       <c r="D12" s="95"/>
       <c r="E12" s="95"/>
       <c r="F12" s="95" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G12" s="95"/>
       <c r="H12" s="95"/>
@@ -7620,7 +7614,7 @@
       <c r="D13" s="96"/>
       <c r="E13" s="96"/>
       <c r="F13" s="96" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G13" s="96"/>
       <c r="H13" s="96"/>
@@ -7756,7 +7750,7 @@
       <c r="B15" s="99"/>
       <c r="C15" s="96"/>
       <c r="D15" s="100" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E15" s="96"/>
       <c r="F15" s="96"/>
@@ -7896,7 +7890,7 @@
       <c r="D17" s="95"/>
       <c r="E17" s="96"/>
       <c r="F17" s="96" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G17" s="96"/>
       <c r="H17" s="96"/>
@@ -7966,7 +7960,7 @@
       <c r="D18" s="95"/>
       <c r="E18" s="96"/>
       <c r="F18" s="96" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G18" s="96"/>
       <c r="H18" s="96"/>
@@ -8464,8 +8458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BO72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV39" sqref="AV39"/>
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB42" sqref="BB42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -8532,7 +8526,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -8548,7 +8542,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -8789,7 +8783,7 @@
     <row r="8" spans="1:67" ht="15.95" customHeight="1">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="24"/>
@@ -13128,7 +13122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BO70"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AY5" sqref="AY5"/>
     </sheetView>
   </sheetViews>
@@ -13196,7 +13190,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -13212,7 +13206,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -13522,7 +13516,7 @@
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
@@ -17354,7 +17348,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -17370,7 +17364,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -20874,7 +20868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BO45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AY5" sqref="AY5"/>
     </sheetView>
   </sheetViews>
@@ -20944,7 +20938,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -20960,7 +20954,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -21935,7 +21929,7 @@
       </c>
       <c r="AO18" s="69"/>
       <c r="AP18" s="68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AQ18" s="70"/>
       <c r="AR18" s="70"/>
@@ -21945,7 +21939,7 @@
       <c r="AV18" s="70"/>
       <c r="AW18" s="69"/>
       <c r="AX18" s="68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AY18" s="70"/>
       <c r="AZ18" s="70"/>
@@ -23361,7 +23355,7 @@
   <dimension ref="A2:BO35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AY5" sqref="AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -23428,7 +23422,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -23444,7 +23438,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -25139,7 +25133,7 @@
   <dimension ref="B1:BM24"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AY5" sqref="AY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -25218,7 +25212,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -25234,7 +25228,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -25458,1049 +25452,1217 @@
       <c r="BF7" s="74"/>
     </row>
     <row r="8" spans="2:65" ht="15.75" customHeight="1">
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="129" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="122"/>
-      <c r="I8" s="122"/>
-      <c r="J8" s="122"/>
-      <c r="K8" s="122"/>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="122" t="s">
+      <c r="D8" s="129"/>
+      <c r="E8" s="129"/>
+      <c r="F8" s="129"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="129"/>
+      <c r="J8" s="129"/>
+      <c r="K8" s="129"/>
+      <c r="L8" s="129"/>
+      <c r="M8" s="129"/>
+      <c r="N8" s="129"/>
+      <c r="O8" s="129" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="123"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="123"/>
-      <c r="T8" s="123"/>
-      <c r="U8" s="125" t="s">
+      <c r="P8" s="130"/>
+      <c r="Q8" s="130"/>
+      <c r="R8" s="130"/>
+      <c r="S8" s="130"/>
+      <c r="T8" s="130"/>
+      <c r="U8" s="132" t="s">
         <v>57</v>
       </c>
-      <c r="V8" s="123"/>
-      <c r="W8" s="122" t="s">
+      <c r="V8" s="130"/>
+      <c r="W8" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="123"/>
-      <c r="Y8" s="125" t="s">
+      <c r="X8" s="130"/>
+      <c r="Y8" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="Z8" s="123"/>
-      <c r="AA8" s="128" t="s">
+      <c r="Z8" s="130"/>
+      <c r="AA8" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="AB8" s="129"/>
-      <c r="AC8" s="129"/>
-      <c r="AD8" s="129"/>
-      <c r="AE8" s="129"/>
-      <c r="AF8" s="129"/>
-      <c r="AG8" s="129"/>
-      <c r="AH8" s="129"/>
-      <c r="AI8" s="129"/>
-      <c r="AJ8" s="129"/>
-      <c r="AK8" s="129"/>
-      <c r="AL8" s="130"/>
-      <c r="AM8" s="122" t="s">
+      <c r="AB8" s="136"/>
+      <c r="AC8" s="136"/>
+      <c r="AD8" s="136"/>
+      <c r="AE8" s="136"/>
+      <c r="AF8" s="136"/>
+      <c r="AG8" s="136"/>
+      <c r="AH8" s="136"/>
+      <c r="AI8" s="136"/>
+      <c r="AJ8" s="136"/>
+      <c r="AK8" s="136"/>
+      <c r="AL8" s="137"/>
+      <c r="AM8" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="AN8" s="123"/>
-      <c r="AO8" s="123"/>
-      <c r="AP8" s="123"/>
-      <c r="AQ8" s="123"/>
-      <c r="AR8" s="123"/>
-      <c r="AS8" s="123"/>
-      <c r="AT8" s="123"/>
-      <c r="AU8" s="123"/>
-      <c r="AV8" s="123"/>
-      <c r="AW8" s="123"/>
-      <c r="AX8" s="126" t="s">
+      <c r="AN8" s="130"/>
+      <c r="AO8" s="130"/>
+      <c r="AP8" s="130"/>
+      <c r="AQ8" s="130"/>
+      <c r="AR8" s="130"/>
+      <c r="AS8" s="130"/>
+      <c r="AT8" s="130"/>
+      <c r="AU8" s="130"/>
+      <c r="AV8" s="130"/>
+      <c r="AW8" s="130"/>
+      <c r="AX8" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="AY8" s="124"/>
-      <c r="AZ8" s="124"/>
-      <c r="BA8" s="124"/>
-      <c r="BB8" s="124"/>
-      <c r="BC8" s="124"/>
-      <c r="BD8" s="124"/>
-      <c r="BE8" s="124"/>
-      <c r="BF8" s="124"/>
+      <c r="AY8" s="131"/>
+      <c r="AZ8" s="131"/>
+      <c r="BA8" s="131"/>
+      <c r="BB8" s="131"/>
+      <c r="BC8" s="131"/>
+      <c r="BD8" s="131"/>
+      <c r="BE8" s="131"/>
+      <c r="BF8" s="131"/>
     </row>
     <row r="9" spans="2:65" ht="15.75" customHeight="1">
-      <c r="B9" s="126"/>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="126"/>
-      <c r="I9" s="126"/>
-      <c r="J9" s="126"/>
-      <c r="K9" s="126"/>
-      <c r="L9" s="126"/>
-      <c r="M9" s="126"/>
-      <c r="N9" s="126"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="124"/>
-      <c r="X9" s="124"/>
-      <c r="Y9" s="124"/>
-      <c r="Z9" s="124"/>
-      <c r="AA9" s="126" t="s">
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="133"/>
+      <c r="J9" s="133"/>
+      <c r="K9" s="133"/>
+      <c r="L9" s="133"/>
+      <c r="M9" s="133"/>
+      <c r="N9" s="133"/>
+      <c r="O9" s="131"/>
+      <c r="P9" s="131"/>
+      <c r="Q9" s="131"/>
+      <c r="R9" s="131"/>
+      <c r="S9" s="131"/>
+      <c r="T9" s="131"/>
+      <c r="U9" s="131"/>
+      <c r="V9" s="131"/>
+      <c r="W9" s="131"/>
+      <c r="X9" s="131"/>
+      <c r="Y9" s="131"/>
+      <c r="Z9" s="131"/>
+      <c r="AA9" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="AB9" s="124"/>
-      <c r="AC9" s="126" t="s">
+      <c r="AB9" s="131"/>
+      <c r="AC9" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="AD9" s="124"/>
-      <c r="AE9" s="127" t="s">
+      <c r="AD9" s="131"/>
+      <c r="AE9" s="134" t="s">
         <v>54</v>
       </c>
-      <c r="AF9" s="124"/>
-      <c r="AG9" s="126" t="s">
+      <c r="AF9" s="131"/>
+      <c r="AG9" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="AH9" s="124"/>
-      <c r="AI9" s="126" t="s">
+      <c r="AH9" s="131"/>
+      <c r="AI9" s="133" t="s">
         <v>55</v>
       </c>
-      <c r="AJ9" s="124"/>
-      <c r="AK9" s="126" t="s">
+      <c r="AJ9" s="131"/>
+      <c r="AK9" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="AL9" s="124"/>
-      <c r="AM9" s="124"/>
-      <c r="AN9" s="124"/>
-      <c r="AO9" s="124"/>
-      <c r="AP9" s="124"/>
-      <c r="AQ9" s="124"/>
-      <c r="AR9" s="124"/>
-      <c r="AS9" s="124"/>
-      <c r="AT9" s="124"/>
-      <c r="AU9" s="124"/>
-      <c r="AV9" s="124"/>
-      <c r="AW9" s="124"/>
-      <c r="AX9" s="124"/>
-      <c r="AY9" s="124"/>
-      <c r="AZ9" s="124"/>
-      <c r="BA9" s="124"/>
-      <c r="BB9" s="124"/>
-      <c r="BC9" s="124"/>
-      <c r="BD9" s="124"/>
-      <c r="BE9" s="124"/>
-      <c r="BF9" s="124"/>
+      <c r="AL9" s="131"/>
+      <c r="AM9" s="131"/>
+      <c r="AN9" s="131"/>
+      <c r="AO9" s="131"/>
+      <c r="AP9" s="131"/>
+      <c r="AQ9" s="131"/>
+      <c r="AR9" s="131"/>
+      <c r="AS9" s="131"/>
+      <c r="AT9" s="131"/>
+      <c r="AU9" s="131"/>
+      <c r="AV9" s="131"/>
+      <c r="AW9" s="131"/>
+      <c r="AX9" s="131"/>
+      <c r="AY9" s="131"/>
+      <c r="AZ9" s="131"/>
+      <c r="BA9" s="131"/>
+      <c r="BB9" s="131"/>
+      <c r="BC9" s="131"/>
+      <c r="BD9" s="131"/>
+      <c r="BE9" s="131"/>
+      <c r="BF9" s="131"/>
     </row>
     <row r="10" spans="2:65" ht="15.75" customHeight="1">
       <c r="B10" s="76"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
-      <c r="N10" s="134"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="133"/>
-      <c r="Q10" s="133"/>
-      <c r="R10" s="133"/>
-      <c r="S10" s="133"/>
-      <c r="T10" s="134"/>
-      <c r="U10" s="135"/>
-      <c r="V10" s="136"/>
-      <c r="W10" s="135"/>
-      <c r="X10" s="136"/>
-      <c r="Y10" s="135"/>
-      <c r="Z10" s="136"/>
-      <c r="AA10" s="135"/>
-      <c r="AB10" s="136"/>
-      <c r="AC10" s="135"/>
-      <c r="AD10" s="136"/>
-      <c r="AE10" s="135"/>
-      <c r="AF10" s="136"/>
-      <c r="AG10" s="135"/>
-      <c r="AH10" s="136"/>
-      <c r="AI10" s="135"/>
-      <c r="AJ10" s="136"/>
-      <c r="AK10" s="135"/>
-      <c r="AL10" s="136"/>
-      <c r="AM10" s="135"/>
-      <c r="AN10" s="137"/>
-      <c r="AO10" s="137"/>
-      <c r="AP10" s="137"/>
-      <c r="AQ10" s="137"/>
-      <c r="AR10" s="137"/>
-      <c r="AS10" s="137"/>
-      <c r="AT10" s="137"/>
-      <c r="AU10" s="137"/>
-      <c r="AV10" s="137"/>
-      <c r="AW10" s="136"/>
-      <c r="AX10" s="131"/>
-      <c r="AY10" s="131"/>
-      <c r="AZ10" s="131"/>
-      <c r="BA10" s="131"/>
-      <c r="BB10" s="131"/>
-      <c r="BC10" s="131"/>
-      <c r="BD10" s="131"/>
-      <c r="BE10" s="131"/>
-      <c r="BF10" s="131"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="127"/>
+      <c r="E10" s="127"/>
+      <c r="F10" s="127"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+      <c r="K10" s="127"/>
+      <c r="L10" s="127"/>
+      <c r="M10" s="127"/>
+      <c r="N10" s="128"/>
+      <c r="O10" s="126"/>
+      <c r="P10" s="127"/>
+      <c r="Q10" s="127"/>
+      <c r="R10" s="127"/>
+      <c r="S10" s="127"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="122"/>
+      <c r="V10" s="123"/>
+      <c r="W10" s="122"/>
+      <c r="X10" s="123"/>
+      <c r="Y10" s="122"/>
+      <c r="Z10" s="123"/>
+      <c r="AA10" s="122"/>
+      <c r="AB10" s="123"/>
+      <c r="AC10" s="122"/>
+      <c r="AD10" s="123"/>
+      <c r="AE10" s="122"/>
+      <c r="AF10" s="123"/>
+      <c r="AG10" s="122"/>
+      <c r="AH10" s="123"/>
+      <c r="AI10" s="122"/>
+      <c r="AJ10" s="123"/>
+      <c r="AK10" s="122"/>
+      <c r="AL10" s="123"/>
+      <c r="AM10" s="122"/>
+      <c r="AN10" s="124"/>
+      <c r="AO10" s="124"/>
+      <c r="AP10" s="124"/>
+      <c r="AQ10" s="124"/>
+      <c r="AR10" s="124"/>
+      <c r="AS10" s="124"/>
+      <c r="AT10" s="124"/>
+      <c r="AU10" s="124"/>
+      <c r="AV10" s="124"/>
+      <c r="AW10" s="123"/>
+      <c r="AX10" s="125"/>
+      <c r="AY10" s="125"/>
+      <c r="AZ10" s="125"/>
+      <c r="BA10" s="125"/>
+      <c r="BB10" s="125"/>
+      <c r="BC10" s="125"/>
+      <c r="BD10" s="125"/>
+      <c r="BE10" s="125"/>
+      <c r="BF10" s="125"/>
     </row>
     <row r="11" spans="2:65" ht="15.75" customHeight="1">
       <c r="B11" s="64"/>
-      <c r="C11" s="132"/>
-      <c r="D11" s="133"/>
-      <c r="E11" s="133"/>
-      <c r="F11" s="133"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="133"/>
-      <c r="I11" s="133"/>
-      <c r="J11" s="133"/>
-      <c r="K11" s="133"/>
-      <c r="L11" s="133"/>
-      <c r="M11" s="133"/>
-      <c r="N11" s="134"/>
-      <c r="O11" s="132"/>
-      <c r="P11" s="133"/>
-      <c r="Q11" s="133"/>
-      <c r="R11" s="133"/>
-      <c r="S11" s="133"/>
-      <c r="T11" s="134"/>
-      <c r="U11" s="135"/>
-      <c r="V11" s="136"/>
-      <c r="W11" s="135"/>
-      <c r="X11" s="136"/>
-      <c r="Y11" s="135"/>
-      <c r="Z11" s="136"/>
-      <c r="AA11" s="135"/>
-      <c r="AB11" s="136"/>
-      <c r="AC11" s="135"/>
-      <c r="AD11" s="136"/>
-      <c r="AE11" s="135"/>
-      <c r="AF11" s="136"/>
-      <c r="AG11" s="135"/>
-      <c r="AH11" s="136"/>
-      <c r="AI11" s="135"/>
-      <c r="AJ11" s="136"/>
-      <c r="AK11" s="135"/>
-      <c r="AL11" s="136"/>
-      <c r="AM11" s="135"/>
-      <c r="AN11" s="137"/>
-      <c r="AO11" s="137"/>
-      <c r="AP11" s="137"/>
-      <c r="AQ11" s="137"/>
-      <c r="AR11" s="137"/>
-      <c r="AS11" s="137"/>
-      <c r="AT11" s="137"/>
-      <c r="AU11" s="137"/>
-      <c r="AV11" s="137"/>
-      <c r="AW11" s="136"/>
-      <c r="AX11" s="131"/>
-      <c r="AY11" s="131"/>
-      <c r="AZ11" s="131"/>
-      <c r="BA11" s="131"/>
-      <c r="BB11" s="131"/>
-      <c r="BC11" s="131"/>
-      <c r="BD11" s="131"/>
-      <c r="BE11" s="131"/>
-      <c r="BF11" s="131"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="127"/>
+      <c r="K11" s="127"/>
+      <c r="L11" s="127"/>
+      <c r="M11" s="127"/>
+      <c r="N11" s="128"/>
+      <c r="O11" s="126"/>
+      <c r="P11" s="127"/>
+      <c r="Q11" s="127"/>
+      <c r="R11" s="127"/>
+      <c r="S11" s="127"/>
+      <c r="T11" s="128"/>
+      <c r="U11" s="122"/>
+      <c r="V11" s="123"/>
+      <c r="W11" s="122"/>
+      <c r="X11" s="123"/>
+      <c r="Y11" s="122"/>
+      <c r="Z11" s="123"/>
+      <c r="AA11" s="122"/>
+      <c r="AB11" s="123"/>
+      <c r="AC11" s="122"/>
+      <c r="AD11" s="123"/>
+      <c r="AE11" s="122"/>
+      <c r="AF11" s="123"/>
+      <c r="AG11" s="122"/>
+      <c r="AH11" s="123"/>
+      <c r="AI11" s="122"/>
+      <c r="AJ11" s="123"/>
+      <c r="AK11" s="122"/>
+      <c r="AL11" s="123"/>
+      <c r="AM11" s="122"/>
+      <c r="AN11" s="124"/>
+      <c r="AO11" s="124"/>
+      <c r="AP11" s="124"/>
+      <c r="AQ11" s="124"/>
+      <c r="AR11" s="124"/>
+      <c r="AS11" s="124"/>
+      <c r="AT11" s="124"/>
+      <c r="AU11" s="124"/>
+      <c r="AV11" s="124"/>
+      <c r="AW11" s="123"/>
+      <c r="AX11" s="125"/>
+      <c r="AY11" s="125"/>
+      <c r="AZ11" s="125"/>
+      <c r="BA11" s="125"/>
+      <c r="BB11" s="125"/>
+      <c r="BC11" s="125"/>
+      <c r="BD11" s="125"/>
+      <c r="BE11" s="125"/>
+      <c r="BF11" s="125"/>
     </row>
     <row r="12" spans="2:65" ht="15.75" customHeight="1">
       <c r="B12" s="64"/>
-      <c r="C12" s="132"/>
-      <c r="D12" s="133"/>
-      <c r="E12" s="133"/>
-      <c r="F12" s="133"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="133"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="132"/>
-      <c r="P12" s="133"/>
-      <c r="Q12" s="133"/>
-      <c r="R12" s="133"/>
-      <c r="S12" s="133"/>
-      <c r="T12" s="134"/>
-      <c r="U12" s="135"/>
-      <c r="V12" s="136"/>
-      <c r="W12" s="135"/>
-      <c r="X12" s="136"/>
-      <c r="Y12" s="135"/>
-      <c r="Z12" s="136"/>
-      <c r="AA12" s="135"/>
-      <c r="AB12" s="136"/>
-      <c r="AC12" s="135"/>
-      <c r="AD12" s="136"/>
-      <c r="AE12" s="135"/>
-      <c r="AF12" s="136"/>
-      <c r="AG12" s="135"/>
-      <c r="AH12" s="136"/>
-      <c r="AI12" s="135"/>
-      <c r="AJ12" s="136"/>
-      <c r="AK12" s="135"/>
-      <c r="AL12" s="136"/>
-      <c r="AM12" s="135"/>
-      <c r="AN12" s="137"/>
-      <c r="AO12" s="137"/>
-      <c r="AP12" s="137"/>
-      <c r="AQ12" s="137"/>
-      <c r="AR12" s="137"/>
-      <c r="AS12" s="137"/>
-      <c r="AT12" s="137"/>
-      <c r="AU12" s="137"/>
-      <c r="AV12" s="137"/>
-      <c r="AW12" s="136"/>
-      <c r="AX12" s="131"/>
-      <c r="AY12" s="131"/>
-      <c r="AZ12" s="131"/>
-      <c r="BA12" s="131"/>
-      <c r="BB12" s="131"/>
-      <c r="BC12" s="131"/>
-      <c r="BD12" s="131"/>
-      <c r="BE12" s="131"/>
-      <c r="BF12" s="131"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="127"/>
+      <c r="E12" s="127"/>
+      <c r="F12" s="127"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+      <c r="K12" s="127"/>
+      <c r="L12" s="127"/>
+      <c r="M12" s="127"/>
+      <c r="N12" s="128"/>
+      <c r="O12" s="126"/>
+      <c r="P12" s="127"/>
+      <c r="Q12" s="127"/>
+      <c r="R12" s="127"/>
+      <c r="S12" s="127"/>
+      <c r="T12" s="128"/>
+      <c r="U12" s="122"/>
+      <c r="V12" s="123"/>
+      <c r="W12" s="122"/>
+      <c r="X12" s="123"/>
+      <c r="Y12" s="122"/>
+      <c r="Z12" s="123"/>
+      <c r="AA12" s="122"/>
+      <c r="AB12" s="123"/>
+      <c r="AC12" s="122"/>
+      <c r="AD12" s="123"/>
+      <c r="AE12" s="122"/>
+      <c r="AF12" s="123"/>
+      <c r="AG12" s="122"/>
+      <c r="AH12" s="123"/>
+      <c r="AI12" s="122"/>
+      <c r="AJ12" s="123"/>
+      <c r="AK12" s="122"/>
+      <c r="AL12" s="123"/>
+      <c r="AM12" s="122"/>
+      <c r="AN12" s="124"/>
+      <c r="AO12" s="124"/>
+      <c r="AP12" s="124"/>
+      <c r="AQ12" s="124"/>
+      <c r="AR12" s="124"/>
+      <c r="AS12" s="124"/>
+      <c r="AT12" s="124"/>
+      <c r="AU12" s="124"/>
+      <c r="AV12" s="124"/>
+      <c r="AW12" s="123"/>
+      <c r="AX12" s="125"/>
+      <c r="AY12" s="125"/>
+      <c r="AZ12" s="125"/>
+      <c r="BA12" s="125"/>
+      <c r="BB12" s="125"/>
+      <c r="BC12" s="125"/>
+      <c r="BD12" s="125"/>
+      <c r="BE12" s="125"/>
+      <c r="BF12" s="125"/>
     </row>
     <row r="13" spans="2:65" ht="15.75" customHeight="1">
       <c r="B13" s="64"/>
-      <c r="C13" s="132"/>
-      <c r="D13" s="133"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="133"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="133"/>
-      <c r="I13" s="133"/>
-      <c r="J13" s="133"/>
-      <c r="K13" s="133"/>
-      <c r="L13" s="133"/>
-      <c r="M13" s="133"/>
-      <c r="N13" s="134"/>
-      <c r="O13" s="132"/>
-      <c r="P13" s="133"/>
-      <c r="Q13" s="133"/>
-      <c r="R13" s="133"/>
-      <c r="S13" s="133"/>
-      <c r="T13" s="134"/>
-      <c r="U13" s="135"/>
-      <c r="V13" s="136"/>
-      <c r="W13" s="135"/>
-      <c r="X13" s="136"/>
-      <c r="Y13" s="135"/>
-      <c r="Z13" s="136"/>
-      <c r="AA13" s="135"/>
-      <c r="AB13" s="136"/>
-      <c r="AC13" s="135"/>
-      <c r="AD13" s="136"/>
-      <c r="AE13" s="135"/>
-      <c r="AF13" s="136"/>
-      <c r="AG13" s="135"/>
-      <c r="AH13" s="136"/>
-      <c r="AI13" s="135"/>
-      <c r="AJ13" s="136"/>
-      <c r="AK13" s="135"/>
-      <c r="AL13" s="136"/>
-      <c r="AM13" s="135"/>
-      <c r="AN13" s="137"/>
-      <c r="AO13" s="137"/>
-      <c r="AP13" s="137"/>
-      <c r="AQ13" s="137"/>
-      <c r="AR13" s="137"/>
-      <c r="AS13" s="137"/>
-      <c r="AT13" s="137"/>
-      <c r="AU13" s="137"/>
-      <c r="AV13" s="137"/>
-      <c r="AW13" s="136"/>
-      <c r="AX13" s="131"/>
-      <c r="AY13" s="131"/>
-      <c r="AZ13" s="131"/>
-      <c r="BA13" s="131"/>
-      <c r="BB13" s="131"/>
-      <c r="BC13" s="131"/>
-      <c r="BD13" s="131"/>
-      <c r="BE13" s="131"/>
-      <c r="BF13" s="131"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
+      <c r="K13" s="127"/>
+      <c r="L13" s="127"/>
+      <c r="M13" s="127"/>
+      <c r="N13" s="128"/>
+      <c r="O13" s="126"/>
+      <c r="P13" s="127"/>
+      <c r="Q13" s="127"/>
+      <c r="R13" s="127"/>
+      <c r="S13" s="127"/>
+      <c r="T13" s="128"/>
+      <c r="U13" s="122"/>
+      <c r="V13" s="123"/>
+      <c r="W13" s="122"/>
+      <c r="X13" s="123"/>
+      <c r="Y13" s="122"/>
+      <c r="Z13" s="123"/>
+      <c r="AA13" s="122"/>
+      <c r="AB13" s="123"/>
+      <c r="AC13" s="122"/>
+      <c r="AD13" s="123"/>
+      <c r="AE13" s="122"/>
+      <c r="AF13" s="123"/>
+      <c r="AG13" s="122"/>
+      <c r="AH13" s="123"/>
+      <c r="AI13" s="122"/>
+      <c r="AJ13" s="123"/>
+      <c r="AK13" s="122"/>
+      <c r="AL13" s="123"/>
+      <c r="AM13" s="122"/>
+      <c r="AN13" s="124"/>
+      <c r="AO13" s="124"/>
+      <c r="AP13" s="124"/>
+      <c r="AQ13" s="124"/>
+      <c r="AR13" s="124"/>
+      <c r="AS13" s="124"/>
+      <c r="AT13" s="124"/>
+      <c r="AU13" s="124"/>
+      <c r="AV13" s="124"/>
+      <c r="AW13" s="123"/>
+      <c r="AX13" s="125"/>
+      <c r="AY13" s="125"/>
+      <c r="AZ13" s="125"/>
+      <c r="BA13" s="125"/>
+      <c r="BB13" s="125"/>
+      <c r="BC13" s="125"/>
+      <c r="BD13" s="125"/>
+      <c r="BE13" s="125"/>
+      <c r="BF13" s="125"/>
     </row>
     <row r="14" spans="2:65" ht="15.75" customHeight="1">
       <c r="B14" s="64"/>
-      <c r="C14" s="132"/>
-      <c r="D14" s="133"/>
-      <c r="E14" s="133"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="133"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="133"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="133"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="134"/>
-      <c r="O14" s="132"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="133"/>
-      <c r="S14" s="133"/>
-      <c r="T14" s="134"/>
-      <c r="U14" s="135"/>
-      <c r="V14" s="136"/>
-      <c r="W14" s="135"/>
-      <c r="X14" s="136"/>
-      <c r="Y14" s="135"/>
-      <c r="Z14" s="136"/>
-      <c r="AA14" s="135"/>
-      <c r="AB14" s="136"/>
-      <c r="AC14" s="135"/>
-      <c r="AD14" s="136"/>
-      <c r="AE14" s="135"/>
-      <c r="AF14" s="136"/>
-      <c r="AG14" s="135"/>
-      <c r="AH14" s="136"/>
-      <c r="AI14" s="135"/>
-      <c r="AJ14" s="136"/>
-      <c r="AK14" s="135"/>
-      <c r="AL14" s="136"/>
-      <c r="AM14" s="135"/>
-      <c r="AN14" s="137"/>
-      <c r="AO14" s="137"/>
-      <c r="AP14" s="137"/>
-      <c r="AQ14" s="137"/>
-      <c r="AR14" s="137"/>
-      <c r="AS14" s="137"/>
-      <c r="AT14" s="137"/>
-      <c r="AU14" s="137"/>
-      <c r="AV14" s="137"/>
-      <c r="AW14" s="136"/>
-      <c r="AX14" s="131"/>
-      <c r="AY14" s="131"/>
-      <c r="AZ14" s="131"/>
-      <c r="BA14" s="131"/>
-      <c r="BB14" s="131"/>
-      <c r="BC14" s="131"/>
-      <c r="BD14" s="131"/>
-      <c r="BE14" s="131"/>
-      <c r="BF14" s="131"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="127"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+      <c r="K14" s="127"/>
+      <c r="L14" s="127"/>
+      <c r="M14" s="127"/>
+      <c r="N14" s="128"/>
+      <c r="O14" s="126"/>
+      <c r="P14" s="127"/>
+      <c r="Q14" s="127"/>
+      <c r="R14" s="127"/>
+      <c r="S14" s="127"/>
+      <c r="T14" s="128"/>
+      <c r="U14" s="122"/>
+      <c r="V14" s="123"/>
+      <c r="W14" s="122"/>
+      <c r="X14" s="123"/>
+      <c r="Y14" s="122"/>
+      <c r="Z14" s="123"/>
+      <c r="AA14" s="122"/>
+      <c r="AB14" s="123"/>
+      <c r="AC14" s="122"/>
+      <c r="AD14" s="123"/>
+      <c r="AE14" s="122"/>
+      <c r="AF14" s="123"/>
+      <c r="AG14" s="122"/>
+      <c r="AH14" s="123"/>
+      <c r="AI14" s="122"/>
+      <c r="AJ14" s="123"/>
+      <c r="AK14" s="122"/>
+      <c r="AL14" s="123"/>
+      <c r="AM14" s="122"/>
+      <c r="AN14" s="124"/>
+      <c r="AO14" s="124"/>
+      <c r="AP14" s="124"/>
+      <c r="AQ14" s="124"/>
+      <c r="AR14" s="124"/>
+      <c r="AS14" s="124"/>
+      <c r="AT14" s="124"/>
+      <c r="AU14" s="124"/>
+      <c r="AV14" s="124"/>
+      <c r="AW14" s="123"/>
+      <c r="AX14" s="125"/>
+      <c r="AY14" s="125"/>
+      <c r="AZ14" s="125"/>
+      <c r="BA14" s="125"/>
+      <c r="BB14" s="125"/>
+      <c r="BC14" s="125"/>
+      <c r="BD14" s="125"/>
+      <c r="BE14" s="125"/>
+      <c r="BF14" s="125"/>
     </row>
     <row r="15" spans="2:65" ht="15.75" customHeight="1">
       <c r="B15" s="64"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="133"/>
-      <c r="E15" s="133"/>
-      <c r="F15" s="133"/>
-      <c r="G15" s="133"/>
-      <c r="H15" s="133"/>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
-      <c r="K15" s="133"/>
-      <c r="L15" s="133"/>
-      <c r="M15" s="133"/>
-      <c r="N15" s="134"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="133"/>
-      <c r="Q15" s="133"/>
-      <c r="R15" s="133"/>
-      <c r="S15" s="133"/>
-      <c r="T15" s="134"/>
-      <c r="U15" s="135"/>
-      <c r="V15" s="136"/>
-      <c r="W15" s="135"/>
-      <c r="X15" s="136"/>
-      <c r="Y15" s="135"/>
-      <c r="Z15" s="136"/>
-      <c r="AA15" s="135"/>
-      <c r="AB15" s="136"/>
-      <c r="AC15" s="135"/>
-      <c r="AD15" s="136"/>
-      <c r="AE15" s="135"/>
-      <c r="AF15" s="136"/>
-      <c r="AG15" s="135"/>
-      <c r="AH15" s="136"/>
-      <c r="AI15" s="135"/>
-      <c r="AJ15" s="136"/>
-      <c r="AK15" s="135"/>
-      <c r="AL15" s="136"/>
-      <c r="AM15" s="135"/>
-      <c r="AN15" s="137"/>
-      <c r="AO15" s="137"/>
-      <c r="AP15" s="137"/>
-      <c r="AQ15" s="137"/>
-      <c r="AR15" s="137"/>
-      <c r="AS15" s="137"/>
-      <c r="AT15" s="137"/>
-      <c r="AU15" s="137"/>
-      <c r="AV15" s="137"/>
-      <c r="AW15" s="136"/>
-      <c r="AX15" s="131"/>
-      <c r="AY15" s="131"/>
-      <c r="AZ15" s="131"/>
-      <c r="BA15" s="131"/>
-      <c r="BB15" s="131"/>
-      <c r="BC15" s="131"/>
-      <c r="BD15" s="131"/>
-      <c r="BE15" s="131"/>
-      <c r="BF15" s="131"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="127"/>
+      <c r="E15" s="127"/>
+      <c r="F15" s="127"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+      <c r="K15" s="127"/>
+      <c r="L15" s="127"/>
+      <c r="M15" s="127"/>
+      <c r="N15" s="128"/>
+      <c r="O15" s="126"/>
+      <c r="P15" s="127"/>
+      <c r="Q15" s="127"/>
+      <c r="R15" s="127"/>
+      <c r="S15" s="127"/>
+      <c r="T15" s="128"/>
+      <c r="U15" s="122"/>
+      <c r="V15" s="123"/>
+      <c r="W15" s="122"/>
+      <c r="X15" s="123"/>
+      <c r="Y15" s="122"/>
+      <c r="Z15" s="123"/>
+      <c r="AA15" s="122"/>
+      <c r="AB15" s="123"/>
+      <c r="AC15" s="122"/>
+      <c r="AD15" s="123"/>
+      <c r="AE15" s="122"/>
+      <c r="AF15" s="123"/>
+      <c r="AG15" s="122"/>
+      <c r="AH15" s="123"/>
+      <c r="AI15" s="122"/>
+      <c r="AJ15" s="123"/>
+      <c r="AK15" s="122"/>
+      <c r="AL15" s="123"/>
+      <c r="AM15" s="122"/>
+      <c r="AN15" s="124"/>
+      <c r="AO15" s="124"/>
+      <c r="AP15" s="124"/>
+      <c r="AQ15" s="124"/>
+      <c r="AR15" s="124"/>
+      <c r="AS15" s="124"/>
+      <c r="AT15" s="124"/>
+      <c r="AU15" s="124"/>
+      <c r="AV15" s="124"/>
+      <c r="AW15" s="123"/>
+      <c r="AX15" s="125"/>
+      <c r="AY15" s="125"/>
+      <c r="AZ15" s="125"/>
+      <c r="BA15" s="125"/>
+      <c r="BB15" s="125"/>
+      <c r="BC15" s="125"/>
+      <c r="BD15" s="125"/>
+      <c r="BE15" s="125"/>
+      <c r="BF15" s="125"/>
     </row>
     <row r="16" spans="2:65" ht="15.75" customHeight="1">
       <c r="B16" s="64"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="133"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-      <c r="I16" s="133"/>
-      <c r="J16" s="133"/>
-      <c r="K16" s="133"/>
-      <c r="L16" s="133"/>
-      <c r="M16" s="133"/>
-      <c r="N16" s="134"/>
-      <c r="O16" s="132"/>
-      <c r="P16" s="133"/>
-      <c r="Q16" s="133"/>
-      <c r="R16" s="133"/>
-      <c r="S16" s="133"/>
-      <c r="T16" s="134"/>
-      <c r="U16" s="135"/>
-      <c r="V16" s="136"/>
-      <c r="W16" s="135"/>
-      <c r="X16" s="136"/>
-      <c r="Y16" s="135"/>
-      <c r="Z16" s="136"/>
-      <c r="AA16" s="135"/>
-      <c r="AB16" s="136"/>
-      <c r="AC16" s="135"/>
-      <c r="AD16" s="136"/>
-      <c r="AE16" s="135"/>
-      <c r="AF16" s="136"/>
-      <c r="AG16" s="135"/>
-      <c r="AH16" s="136"/>
-      <c r="AI16" s="135"/>
-      <c r="AJ16" s="136"/>
-      <c r="AK16" s="135"/>
-      <c r="AL16" s="136"/>
-      <c r="AM16" s="135"/>
-      <c r="AN16" s="137"/>
-      <c r="AO16" s="137"/>
-      <c r="AP16" s="137"/>
-      <c r="AQ16" s="137"/>
-      <c r="AR16" s="137"/>
-      <c r="AS16" s="137"/>
-      <c r="AT16" s="137"/>
-      <c r="AU16" s="137"/>
-      <c r="AV16" s="137"/>
-      <c r="AW16" s="136"/>
-      <c r="AX16" s="131"/>
-      <c r="AY16" s="131"/>
-      <c r="AZ16" s="131"/>
-      <c r="BA16" s="131"/>
-      <c r="BB16" s="131"/>
-      <c r="BC16" s="131"/>
-      <c r="BD16" s="131"/>
-      <c r="BE16" s="131"/>
-      <c r="BF16" s="131"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="127"/>
+      <c r="E16" s="127"/>
+      <c r="F16" s="127"/>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="127"/>
+      <c r="L16" s="127"/>
+      <c r="M16" s="127"/>
+      <c r="N16" s="128"/>
+      <c r="O16" s="126"/>
+      <c r="P16" s="127"/>
+      <c r="Q16" s="127"/>
+      <c r="R16" s="127"/>
+      <c r="S16" s="127"/>
+      <c r="T16" s="128"/>
+      <c r="U16" s="122"/>
+      <c r="V16" s="123"/>
+      <c r="W16" s="122"/>
+      <c r="X16" s="123"/>
+      <c r="Y16" s="122"/>
+      <c r="Z16" s="123"/>
+      <c r="AA16" s="122"/>
+      <c r="AB16" s="123"/>
+      <c r="AC16" s="122"/>
+      <c r="AD16" s="123"/>
+      <c r="AE16" s="122"/>
+      <c r="AF16" s="123"/>
+      <c r="AG16" s="122"/>
+      <c r="AH16" s="123"/>
+      <c r="AI16" s="122"/>
+      <c r="AJ16" s="123"/>
+      <c r="AK16" s="122"/>
+      <c r="AL16" s="123"/>
+      <c r="AM16" s="122"/>
+      <c r="AN16" s="124"/>
+      <c r="AO16" s="124"/>
+      <c r="AP16" s="124"/>
+      <c r="AQ16" s="124"/>
+      <c r="AR16" s="124"/>
+      <c r="AS16" s="124"/>
+      <c r="AT16" s="124"/>
+      <c r="AU16" s="124"/>
+      <c r="AV16" s="124"/>
+      <c r="AW16" s="123"/>
+      <c r="AX16" s="125"/>
+      <c r="AY16" s="125"/>
+      <c r="AZ16" s="125"/>
+      <c r="BA16" s="125"/>
+      <c r="BB16" s="125"/>
+      <c r="BC16" s="125"/>
+      <c r="BD16" s="125"/>
+      <c r="BE16" s="125"/>
+      <c r="BF16" s="125"/>
     </row>
     <row r="17" spans="2:58" ht="15.75" customHeight="1">
       <c r="B17" s="64"/>
-      <c r="C17" s="132"/>
-      <c r="D17" s="133"/>
-      <c r="E17" s="133"/>
-      <c r="F17" s="133"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="133"/>
-      <c r="I17" s="133"/>
-      <c r="J17" s="133"/>
-      <c r="K17" s="133"/>
-      <c r="L17" s="133"/>
-      <c r="M17" s="133"/>
-      <c r="N17" s="134"/>
-      <c r="O17" s="132"/>
-      <c r="P17" s="133"/>
-      <c r="Q17" s="133"/>
-      <c r="R17" s="133"/>
-      <c r="S17" s="133"/>
-      <c r="T17" s="134"/>
-      <c r="U17" s="135"/>
-      <c r="V17" s="136"/>
-      <c r="W17" s="135"/>
-      <c r="X17" s="136"/>
-      <c r="Y17" s="135"/>
-      <c r="Z17" s="136"/>
-      <c r="AA17" s="135"/>
-      <c r="AB17" s="136"/>
-      <c r="AC17" s="135"/>
-      <c r="AD17" s="136"/>
-      <c r="AE17" s="135"/>
-      <c r="AF17" s="136"/>
-      <c r="AG17" s="135"/>
-      <c r="AH17" s="136"/>
-      <c r="AI17" s="135"/>
-      <c r="AJ17" s="136"/>
-      <c r="AK17" s="135"/>
-      <c r="AL17" s="136"/>
-      <c r="AM17" s="135"/>
-      <c r="AN17" s="137"/>
-      <c r="AO17" s="137"/>
-      <c r="AP17" s="137"/>
-      <c r="AQ17" s="137"/>
-      <c r="AR17" s="137"/>
-      <c r="AS17" s="137"/>
-      <c r="AT17" s="137"/>
-      <c r="AU17" s="137"/>
-      <c r="AV17" s="137"/>
-      <c r="AW17" s="136"/>
-      <c r="AX17" s="131"/>
-      <c r="AY17" s="131"/>
-      <c r="AZ17" s="131"/>
-      <c r="BA17" s="131"/>
-      <c r="BB17" s="131"/>
-      <c r="BC17" s="131"/>
-      <c r="BD17" s="131"/>
-      <c r="BE17" s="131"/>
-      <c r="BF17" s="131"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="127"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="127"/>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+      <c r="K17" s="127"/>
+      <c r="L17" s="127"/>
+      <c r="M17" s="127"/>
+      <c r="N17" s="128"/>
+      <c r="O17" s="126"/>
+      <c r="P17" s="127"/>
+      <c r="Q17" s="127"/>
+      <c r="R17" s="127"/>
+      <c r="S17" s="127"/>
+      <c r="T17" s="128"/>
+      <c r="U17" s="122"/>
+      <c r="V17" s="123"/>
+      <c r="W17" s="122"/>
+      <c r="X17" s="123"/>
+      <c r="Y17" s="122"/>
+      <c r="Z17" s="123"/>
+      <c r="AA17" s="122"/>
+      <c r="AB17" s="123"/>
+      <c r="AC17" s="122"/>
+      <c r="AD17" s="123"/>
+      <c r="AE17" s="122"/>
+      <c r="AF17" s="123"/>
+      <c r="AG17" s="122"/>
+      <c r="AH17" s="123"/>
+      <c r="AI17" s="122"/>
+      <c r="AJ17" s="123"/>
+      <c r="AK17" s="122"/>
+      <c r="AL17" s="123"/>
+      <c r="AM17" s="122"/>
+      <c r="AN17" s="124"/>
+      <c r="AO17" s="124"/>
+      <c r="AP17" s="124"/>
+      <c r="AQ17" s="124"/>
+      <c r="AR17" s="124"/>
+      <c r="AS17" s="124"/>
+      <c r="AT17" s="124"/>
+      <c r="AU17" s="124"/>
+      <c r="AV17" s="124"/>
+      <c r="AW17" s="123"/>
+      <c r="AX17" s="125"/>
+      <c r="AY17" s="125"/>
+      <c r="AZ17" s="125"/>
+      <c r="BA17" s="125"/>
+      <c r="BB17" s="125"/>
+      <c r="BC17" s="125"/>
+      <c r="BD17" s="125"/>
+      <c r="BE17" s="125"/>
+      <c r="BF17" s="125"/>
     </row>
     <row r="18" spans="2:58" ht="15.75" customHeight="1">
       <c r="B18" s="64"/>
-      <c r="C18" s="132"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="133"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="133"/>
-      <c r="J18" s="133"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="133"/>
-      <c r="N18" s="134"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="133"/>
-      <c r="Q18" s="133"/>
-      <c r="R18" s="133"/>
-      <c r="S18" s="133"/>
-      <c r="T18" s="134"/>
-      <c r="U18" s="135"/>
-      <c r="V18" s="136"/>
-      <c r="W18" s="135"/>
-      <c r="X18" s="136"/>
-      <c r="Y18" s="135"/>
-      <c r="Z18" s="136"/>
-      <c r="AA18" s="135"/>
-      <c r="AB18" s="136"/>
-      <c r="AC18" s="135"/>
-      <c r="AD18" s="136"/>
-      <c r="AE18" s="135"/>
-      <c r="AF18" s="136"/>
-      <c r="AG18" s="135"/>
-      <c r="AH18" s="136"/>
-      <c r="AI18" s="135"/>
-      <c r="AJ18" s="136"/>
-      <c r="AK18" s="135"/>
-      <c r="AL18" s="136"/>
-      <c r="AM18" s="135"/>
-      <c r="AN18" s="137"/>
-      <c r="AO18" s="137"/>
-      <c r="AP18" s="137"/>
-      <c r="AQ18" s="137"/>
-      <c r="AR18" s="137"/>
-      <c r="AS18" s="137"/>
-      <c r="AT18" s="137"/>
-      <c r="AU18" s="137"/>
-      <c r="AV18" s="137"/>
-      <c r="AW18" s="136"/>
-      <c r="AX18" s="131"/>
-      <c r="AY18" s="131"/>
-      <c r="AZ18" s="131"/>
-      <c r="BA18" s="131"/>
-      <c r="BB18" s="131"/>
-      <c r="BC18" s="131"/>
-      <c r="BD18" s="131"/>
-      <c r="BE18" s="131"/>
-      <c r="BF18" s="131"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="127"/>
+      <c r="E18" s="127"/>
+      <c r="F18" s="127"/>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
+      <c r="K18" s="127"/>
+      <c r="L18" s="127"/>
+      <c r="M18" s="127"/>
+      <c r="N18" s="128"/>
+      <c r="O18" s="126"/>
+      <c r="P18" s="127"/>
+      <c r="Q18" s="127"/>
+      <c r="R18" s="127"/>
+      <c r="S18" s="127"/>
+      <c r="T18" s="128"/>
+      <c r="U18" s="122"/>
+      <c r="V18" s="123"/>
+      <c r="W18" s="122"/>
+      <c r="X18" s="123"/>
+      <c r="Y18" s="122"/>
+      <c r="Z18" s="123"/>
+      <c r="AA18" s="122"/>
+      <c r="AB18" s="123"/>
+      <c r="AC18" s="122"/>
+      <c r="AD18" s="123"/>
+      <c r="AE18" s="122"/>
+      <c r="AF18" s="123"/>
+      <c r="AG18" s="122"/>
+      <c r="AH18" s="123"/>
+      <c r="AI18" s="122"/>
+      <c r="AJ18" s="123"/>
+      <c r="AK18" s="122"/>
+      <c r="AL18" s="123"/>
+      <c r="AM18" s="122"/>
+      <c r="AN18" s="124"/>
+      <c r="AO18" s="124"/>
+      <c r="AP18" s="124"/>
+      <c r="AQ18" s="124"/>
+      <c r="AR18" s="124"/>
+      <c r="AS18" s="124"/>
+      <c r="AT18" s="124"/>
+      <c r="AU18" s="124"/>
+      <c r="AV18" s="124"/>
+      <c r="AW18" s="123"/>
+      <c r="AX18" s="125"/>
+      <c r="AY18" s="125"/>
+      <c r="AZ18" s="125"/>
+      <c r="BA18" s="125"/>
+      <c r="BB18" s="125"/>
+      <c r="BC18" s="125"/>
+      <c r="BD18" s="125"/>
+      <c r="BE18" s="125"/>
+      <c r="BF18" s="125"/>
     </row>
     <row r="19" spans="2:58" ht="15.75" customHeight="1">
       <c r="B19" s="64"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133"/>
-      <c r="F19" s="133"/>
-      <c r="G19" s="133"/>
-      <c r="H19" s="133"/>
-      <c r="I19" s="133"/>
-      <c r="J19" s="133"/>
-      <c r="K19" s="133"/>
-      <c r="L19" s="133"/>
-      <c r="M19" s="133"/>
-      <c r="N19" s="134"/>
-      <c r="O19" s="132"/>
-      <c r="P19" s="133"/>
-      <c r="Q19" s="133"/>
-      <c r="R19" s="133"/>
-      <c r="S19" s="133"/>
-      <c r="T19" s="134"/>
-      <c r="U19" s="135"/>
-      <c r="V19" s="136"/>
-      <c r="W19" s="135"/>
-      <c r="X19" s="136"/>
-      <c r="Y19" s="135"/>
-      <c r="Z19" s="136"/>
-      <c r="AA19" s="135"/>
-      <c r="AB19" s="136"/>
-      <c r="AC19" s="135"/>
-      <c r="AD19" s="136"/>
-      <c r="AE19" s="135"/>
-      <c r="AF19" s="136"/>
-      <c r="AG19" s="135"/>
-      <c r="AH19" s="136"/>
-      <c r="AI19" s="135"/>
-      <c r="AJ19" s="136"/>
-      <c r="AK19" s="135"/>
-      <c r="AL19" s="136"/>
-      <c r="AM19" s="135"/>
-      <c r="AN19" s="137"/>
-      <c r="AO19" s="137"/>
-      <c r="AP19" s="137"/>
-      <c r="AQ19" s="137"/>
-      <c r="AR19" s="137"/>
-      <c r="AS19" s="137"/>
-      <c r="AT19" s="137"/>
-      <c r="AU19" s="137"/>
-      <c r="AV19" s="137"/>
-      <c r="AW19" s="136"/>
-      <c r="AX19" s="131"/>
-      <c r="AY19" s="131"/>
-      <c r="AZ19" s="131"/>
-      <c r="BA19" s="131"/>
-      <c r="BB19" s="131"/>
-      <c r="BC19" s="131"/>
-      <c r="BD19" s="131"/>
-      <c r="BE19" s="131"/>
-      <c r="BF19" s="131"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="127"/>
+      <c r="E19" s="127"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="127"/>
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
+      <c r="K19" s="127"/>
+      <c r="L19" s="127"/>
+      <c r="M19" s="127"/>
+      <c r="N19" s="128"/>
+      <c r="O19" s="126"/>
+      <c r="P19" s="127"/>
+      <c r="Q19" s="127"/>
+      <c r="R19" s="127"/>
+      <c r="S19" s="127"/>
+      <c r="T19" s="128"/>
+      <c r="U19" s="122"/>
+      <c r="V19" s="123"/>
+      <c r="W19" s="122"/>
+      <c r="X19" s="123"/>
+      <c r="Y19" s="122"/>
+      <c r="Z19" s="123"/>
+      <c r="AA19" s="122"/>
+      <c r="AB19" s="123"/>
+      <c r="AC19" s="122"/>
+      <c r="AD19" s="123"/>
+      <c r="AE19" s="122"/>
+      <c r="AF19" s="123"/>
+      <c r="AG19" s="122"/>
+      <c r="AH19" s="123"/>
+      <c r="AI19" s="122"/>
+      <c r="AJ19" s="123"/>
+      <c r="AK19" s="122"/>
+      <c r="AL19" s="123"/>
+      <c r="AM19" s="122"/>
+      <c r="AN19" s="124"/>
+      <c r="AO19" s="124"/>
+      <c r="AP19" s="124"/>
+      <c r="AQ19" s="124"/>
+      <c r="AR19" s="124"/>
+      <c r="AS19" s="124"/>
+      <c r="AT19" s="124"/>
+      <c r="AU19" s="124"/>
+      <c r="AV19" s="124"/>
+      <c r="AW19" s="123"/>
+      <c r="AX19" s="125"/>
+      <c r="AY19" s="125"/>
+      <c r="AZ19" s="125"/>
+      <c r="BA19" s="125"/>
+      <c r="BB19" s="125"/>
+      <c r="BC19" s="125"/>
+      <c r="BD19" s="125"/>
+      <c r="BE19" s="125"/>
+      <c r="BF19" s="125"/>
     </row>
     <row r="20" spans="2:58" ht="15.75" customHeight="1">
       <c r="B20" s="64"/>
-      <c r="C20" s="132"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="133"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="133"/>
-      <c r="L20" s="133"/>
-      <c r="M20" s="133"/>
-      <c r="N20" s="134"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="133"/>
-      <c r="Q20" s="133"/>
-      <c r="R20" s="133"/>
-      <c r="S20" s="133"/>
-      <c r="T20" s="134"/>
-      <c r="U20" s="135"/>
-      <c r="V20" s="136"/>
-      <c r="W20" s="135"/>
-      <c r="X20" s="136"/>
-      <c r="Y20" s="135"/>
-      <c r="Z20" s="136"/>
-      <c r="AA20" s="135"/>
-      <c r="AB20" s="136"/>
-      <c r="AC20" s="135"/>
-      <c r="AD20" s="136"/>
-      <c r="AE20" s="135"/>
-      <c r="AF20" s="136"/>
-      <c r="AG20" s="135"/>
-      <c r="AH20" s="136"/>
-      <c r="AI20" s="135"/>
-      <c r="AJ20" s="136"/>
-      <c r="AK20" s="135"/>
-      <c r="AL20" s="136"/>
-      <c r="AM20" s="135"/>
-      <c r="AN20" s="137"/>
-      <c r="AO20" s="137"/>
-      <c r="AP20" s="137"/>
-      <c r="AQ20" s="137"/>
-      <c r="AR20" s="137"/>
-      <c r="AS20" s="137"/>
-      <c r="AT20" s="137"/>
-      <c r="AU20" s="137"/>
-      <c r="AV20" s="137"/>
-      <c r="AW20" s="136"/>
-      <c r="AX20" s="131"/>
-      <c r="AY20" s="131"/>
-      <c r="AZ20" s="131"/>
-      <c r="BA20" s="131"/>
-      <c r="BB20" s="131"/>
-      <c r="BC20" s="131"/>
-      <c r="BD20" s="131"/>
-      <c r="BE20" s="131"/>
-      <c r="BF20" s="131"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="127"/>
+      <c r="F20" s="127"/>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
+      <c r="K20" s="127"/>
+      <c r="L20" s="127"/>
+      <c r="M20" s="127"/>
+      <c r="N20" s="128"/>
+      <c r="O20" s="126"/>
+      <c r="P20" s="127"/>
+      <c r="Q20" s="127"/>
+      <c r="R20" s="127"/>
+      <c r="S20" s="127"/>
+      <c r="T20" s="128"/>
+      <c r="U20" s="122"/>
+      <c r="V20" s="123"/>
+      <c r="W20" s="122"/>
+      <c r="X20" s="123"/>
+      <c r="Y20" s="122"/>
+      <c r="Z20" s="123"/>
+      <c r="AA20" s="122"/>
+      <c r="AB20" s="123"/>
+      <c r="AC20" s="122"/>
+      <c r="AD20" s="123"/>
+      <c r="AE20" s="122"/>
+      <c r="AF20" s="123"/>
+      <c r="AG20" s="122"/>
+      <c r="AH20" s="123"/>
+      <c r="AI20" s="122"/>
+      <c r="AJ20" s="123"/>
+      <c r="AK20" s="122"/>
+      <c r="AL20" s="123"/>
+      <c r="AM20" s="122"/>
+      <c r="AN20" s="124"/>
+      <c r="AO20" s="124"/>
+      <c r="AP20" s="124"/>
+      <c r="AQ20" s="124"/>
+      <c r="AR20" s="124"/>
+      <c r="AS20" s="124"/>
+      <c r="AT20" s="124"/>
+      <c r="AU20" s="124"/>
+      <c r="AV20" s="124"/>
+      <c r="AW20" s="123"/>
+      <c r="AX20" s="125"/>
+      <c r="AY20" s="125"/>
+      <c r="AZ20" s="125"/>
+      <c r="BA20" s="125"/>
+      <c r="BB20" s="125"/>
+      <c r="BC20" s="125"/>
+      <c r="BD20" s="125"/>
+      <c r="BE20" s="125"/>
+      <c r="BF20" s="125"/>
     </row>
     <row r="21" spans="2:58" ht="15.75" customHeight="1">
       <c r="B21" s="64"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="133"/>
-      <c r="E21" s="133"/>
-      <c r="F21" s="133"/>
-      <c r="G21" s="133"/>
-      <c r="H21" s="133"/>
-      <c r="I21" s="133"/>
-      <c r="J21" s="133"/>
-      <c r="K21" s="133"/>
-      <c r="L21" s="133"/>
-      <c r="M21" s="133"/>
-      <c r="N21" s="134"/>
-      <c r="O21" s="132"/>
-      <c r="P21" s="133"/>
-      <c r="Q21" s="133"/>
-      <c r="R21" s="133"/>
-      <c r="S21" s="133"/>
-      <c r="T21" s="134"/>
-      <c r="U21" s="135"/>
-      <c r="V21" s="136"/>
-      <c r="W21" s="135"/>
-      <c r="X21" s="136"/>
-      <c r="Y21" s="135"/>
-      <c r="Z21" s="136"/>
-      <c r="AA21" s="135"/>
-      <c r="AB21" s="136"/>
-      <c r="AC21" s="135"/>
-      <c r="AD21" s="136"/>
-      <c r="AE21" s="135"/>
-      <c r="AF21" s="136"/>
-      <c r="AG21" s="135"/>
-      <c r="AH21" s="136"/>
-      <c r="AI21" s="135"/>
-      <c r="AJ21" s="136"/>
-      <c r="AK21" s="135"/>
-      <c r="AL21" s="136"/>
-      <c r="AM21" s="135"/>
-      <c r="AN21" s="137"/>
-      <c r="AO21" s="137"/>
-      <c r="AP21" s="137"/>
-      <c r="AQ21" s="137"/>
-      <c r="AR21" s="137"/>
-      <c r="AS21" s="137"/>
-      <c r="AT21" s="137"/>
-      <c r="AU21" s="137"/>
-      <c r="AV21" s="137"/>
-      <c r="AW21" s="136"/>
-      <c r="AX21" s="131"/>
-      <c r="AY21" s="131"/>
-      <c r="AZ21" s="131"/>
-      <c r="BA21" s="131"/>
-      <c r="BB21" s="131"/>
-      <c r="BC21" s="131"/>
-      <c r="BD21" s="131"/>
-      <c r="BE21" s="131"/>
-      <c r="BF21" s="131"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="127"/>
+      <c r="M21" s="127"/>
+      <c r="N21" s="128"/>
+      <c r="O21" s="126"/>
+      <c r="P21" s="127"/>
+      <c r="Q21" s="127"/>
+      <c r="R21" s="127"/>
+      <c r="S21" s="127"/>
+      <c r="T21" s="128"/>
+      <c r="U21" s="122"/>
+      <c r="V21" s="123"/>
+      <c r="W21" s="122"/>
+      <c r="X21" s="123"/>
+      <c r="Y21" s="122"/>
+      <c r="Z21" s="123"/>
+      <c r="AA21" s="122"/>
+      <c r="AB21" s="123"/>
+      <c r="AC21" s="122"/>
+      <c r="AD21" s="123"/>
+      <c r="AE21" s="122"/>
+      <c r="AF21" s="123"/>
+      <c r="AG21" s="122"/>
+      <c r="AH21" s="123"/>
+      <c r="AI21" s="122"/>
+      <c r="AJ21" s="123"/>
+      <c r="AK21" s="122"/>
+      <c r="AL21" s="123"/>
+      <c r="AM21" s="122"/>
+      <c r="AN21" s="124"/>
+      <c r="AO21" s="124"/>
+      <c r="AP21" s="124"/>
+      <c r="AQ21" s="124"/>
+      <c r="AR21" s="124"/>
+      <c r="AS21" s="124"/>
+      <c r="AT21" s="124"/>
+      <c r="AU21" s="124"/>
+      <c r="AV21" s="124"/>
+      <c r="AW21" s="123"/>
+      <c r="AX21" s="125"/>
+      <c r="AY21" s="125"/>
+      <c r="AZ21" s="125"/>
+      <c r="BA21" s="125"/>
+      <c r="BB21" s="125"/>
+      <c r="BC21" s="125"/>
+      <c r="BD21" s="125"/>
+      <c r="BE21" s="125"/>
+      <c r="BF21" s="125"/>
     </row>
     <row r="22" spans="2:58" ht="15.75" customHeight="1">
       <c r="B22" s="64"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="133"/>
-      <c r="K22" s="133"/>
-      <c r="L22" s="133"/>
-      <c r="M22" s="133"/>
-      <c r="N22" s="134"/>
-      <c r="O22" s="132"/>
-      <c r="P22" s="133"/>
-      <c r="Q22" s="133"/>
-      <c r="R22" s="133"/>
-      <c r="S22" s="133"/>
-      <c r="T22" s="134"/>
-      <c r="U22" s="135"/>
-      <c r="V22" s="136"/>
-      <c r="W22" s="135"/>
-      <c r="X22" s="136"/>
-      <c r="Y22" s="135"/>
-      <c r="Z22" s="136"/>
-      <c r="AA22" s="135"/>
-      <c r="AB22" s="136"/>
-      <c r="AC22" s="135"/>
-      <c r="AD22" s="136"/>
-      <c r="AE22" s="135"/>
-      <c r="AF22" s="136"/>
-      <c r="AG22" s="135"/>
-      <c r="AH22" s="136"/>
-      <c r="AI22" s="135"/>
-      <c r="AJ22" s="136"/>
-      <c r="AK22" s="135"/>
-      <c r="AL22" s="136"/>
-      <c r="AM22" s="135"/>
-      <c r="AN22" s="137"/>
-      <c r="AO22" s="137"/>
-      <c r="AP22" s="137"/>
-      <c r="AQ22" s="137"/>
-      <c r="AR22" s="137"/>
-      <c r="AS22" s="137"/>
-      <c r="AT22" s="137"/>
-      <c r="AU22" s="137"/>
-      <c r="AV22" s="137"/>
-      <c r="AW22" s="136"/>
-      <c r="AX22" s="131"/>
-      <c r="AY22" s="131"/>
-      <c r="AZ22" s="131"/>
-      <c r="BA22" s="131"/>
-      <c r="BB22" s="131"/>
-      <c r="BC22" s="131"/>
-      <c r="BD22" s="131"/>
-      <c r="BE22" s="131"/>
-      <c r="BF22" s="131"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="127"/>
+      <c r="K22" s="127"/>
+      <c r="L22" s="127"/>
+      <c r="M22" s="127"/>
+      <c r="N22" s="128"/>
+      <c r="O22" s="126"/>
+      <c r="P22" s="127"/>
+      <c r="Q22" s="127"/>
+      <c r="R22" s="127"/>
+      <c r="S22" s="127"/>
+      <c r="T22" s="128"/>
+      <c r="U22" s="122"/>
+      <c r="V22" s="123"/>
+      <c r="W22" s="122"/>
+      <c r="X22" s="123"/>
+      <c r="Y22" s="122"/>
+      <c r="Z22" s="123"/>
+      <c r="AA22" s="122"/>
+      <c r="AB22" s="123"/>
+      <c r="AC22" s="122"/>
+      <c r="AD22" s="123"/>
+      <c r="AE22" s="122"/>
+      <c r="AF22" s="123"/>
+      <c r="AG22" s="122"/>
+      <c r="AH22" s="123"/>
+      <c r="AI22" s="122"/>
+      <c r="AJ22" s="123"/>
+      <c r="AK22" s="122"/>
+      <c r="AL22" s="123"/>
+      <c r="AM22" s="122"/>
+      <c r="AN22" s="124"/>
+      <c r="AO22" s="124"/>
+      <c r="AP22" s="124"/>
+      <c r="AQ22" s="124"/>
+      <c r="AR22" s="124"/>
+      <c r="AS22" s="124"/>
+      <c r="AT22" s="124"/>
+      <c r="AU22" s="124"/>
+      <c r="AV22" s="124"/>
+      <c r="AW22" s="123"/>
+      <c r="AX22" s="125"/>
+      <c r="AY22" s="125"/>
+      <c r="AZ22" s="125"/>
+      <c r="BA22" s="125"/>
+      <c r="BB22" s="125"/>
+      <c r="BC22" s="125"/>
+      <c r="BD22" s="125"/>
+      <c r="BE22" s="125"/>
+      <c r="BF22" s="125"/>
     </row>
     <row r="23" spans="2:58" ht="15.75" customHeight="1">
       <c r="B23" s="64"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="133"/>
-      <c r="G23" s="133"/>
-      <c r="H23" s="133"/>
-      <c r="I23" s="133"/>
-      <c r="J23" s="133"/>
-      <c r="K23" s="133"/>
-      <c r="L23" s="133"/>
-      <c r="M23" s="133"/>
-      <c r="N23" s="134"/>
-      <c r="O23" s="132"/>
-      <c r="P23" s="133"/>
-      <c r="Q23" s="133"/>
-      <c r="R23" s="133"/>
-      <c r="S23" s="133"/>
-      <c r="T23" s="134"/>
-      <c r="U23" s="135"/>
-      <c r="V23" s="136"/>
-      <c r="W23" s="135"/>
-      <c r="X23" s="136"/>
-      <c r="Y23" s="135"/>
-      <c r="Z23" s="136"/>
-      <c r="AA23" s="135"/>
-      <c r="AB23" s="136"/>
-      <c r="AC23" s="135"/>
-      <c r="AD23" s="136"/>
-      <c r="AE23" s="135"/>
-      <c r="AF23" s="136"/>
-      <c r="AG23" s="135"/>
-      <c r="AH23" s="136"/>
-      <c r="AI23" s="135"/>
-      <c r="AJ23" s="136"/>
-      <c r="AK23" s="135"/>
-      <c r="AL23" s="136"/>
-      <c r="AM23" s="135"/>
-      <c r="AN23" s="137"/>
-      <c r="AO23" s="137"/>
-      <c r="AP23" s="137"/>
-      <c r="AQ23" s="137"/>
-      <c r="AR23" s="137"/>
-      <c r="AS23" s="137"/>
-      <c r="AT23" s="137"/>
-      <c r="AU23" s="137"/>
-      <c r="AV23" s="137"/>
-      <c r="AW23" s="136"/>
-      <c r="AX23" s="131"/>
-      <c r="AY23" s="131"/>
-      <c r="AZ23" s="131"/>
-      <c r="BA23" s="131"/>
-      <c r="BB23" s="131"/>
-      <c r="BC23" s="131"/>
-      <c r="BD23" s="131"/>
-      <c r="BE23" s="131"/>
-      <c r="BF23" s="131"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="127"/>
+      <c r="L23" s="127"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="128"/>
+      <c r="O23" s="126"/>
+      <c r="P23" s="127"/>
+      <c r="Q23" s="127"/>
+      <c r="R23" s="127"/>
+      <c r="S23" s="127"/>
+      <c r="T23" s="128"/>
+      <c r="U23" s="122"/>
+      <c r="V23" s="123"/>
+      <c r="W23" s="122"/>
+      <c r="X23" s="123"/>
+      <c r="Y23" s="122"/>
+      <c r="Z23" s="123"/>
+      <c r="AA23" s="122"/>
+      <c r="AB23" s="123"/>
+      <c r="AC23" s="122"/>
+      <c r="AD23" s="123"/>
+      <c r="AE23" s="122"/>
+      <c r="AF23" s="123"/>
+      <c r="AG23" s="122"/>
+      <c r="AH23" s="123"/>
+      <c r="AI23" s="122"/>
+      <c r="AJ23" s="123"/>
+      <c r="AK23" s="122"/>
+      <c r="AL23" s="123"/>
+      <c r="AM23" s="122"/>
+      <c r="AN23" s="124"/>
+      <c r="AO23" s="124"/>
+      <c r="AP23" s="124"/>
+      <c r="AQ23" s="124"/>
+      <c r="AR23" s="124"/>
+      <c r="AS23" s="124"/>
+      <c r="AT23" s="124"/>
+      <c r="AU23" s="124"/>
+      <c r="AV23" s="124"/>
+      <c r="AW23" s="123"/>
+      <c r="AX23" s="125"/>
+      <c r="AY23" s="125"/>
+      <c r="AZ23" s="125"/>
+      <c r="BA23" s="125"/>
+      <c r="BB23" s="125"/>
+      <c r="BC23" s="125"/>
+      <c r="BD23" s="125"/>
+      <c r="BE23" s="125"/>
+      <c r="BF23" s="125"/>
     </row>
     <row r="24" spans="2:58" ht="15.75" customHeight="1">
       <c r="B24" s="64"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
-      <c r="G24" s="133"/>
-      <c r="H24" s="133"/>
-      <c r="I24" s="133"/>
-      <c r="J24" s="133"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="133"/>
-      <c r="M24" s="133"/>
-      <c r="N24" s="134"/>
-      <c r="O24" s="132"/>
-      <c r="P24" s="133"/>
-      <c r="Q24" s="133"/>
-      <c r="R24" s="133"/>
-      <c r="S24" s="133"/>
-      <c r="T24" s="134"/>
-      <c r="U24" s="135"/>
-      <c r="V24" s="136"/>
-      <c r="W24" s="135"/>
-      <c r="X24" s="136"/>
-      <c r="Y24" s="135"/>
-      <c r="Z24" s="136"/>
-      <c r="AA24" s="135"/>
-      <c r="AB24" s="136"/>
-      <c r="AC24" s="135"/>
-      <c r="AD24" s="136"/>
-      <c r="AE24" s="135"/>
-      <c r="AF24" s="136"/>
-      <c r="AG24" s="135"/>
-      <c r="AH24" s="136"/>
-      <c r="AI24" s="135"/>
-      <c r="AJ24" s="136"/>
-      <c r="AK24" s="135"/>
-      <c r="AL24" s="136"/>
-      <c r="AM24" s="135"/>
-      <c r="AN24" s="137"/>
-      <c r="AO24" s="137"/>
-      <c r="AP24" s="137"/>
-      <c r="AQ24" s="137"/>
-      <c r="AR24" s="137"/>
-      <c r="AS24" s="137"/>
-      <c r="AT24" s="137"/>
-      <c r="AU24" s="137"/>
-      <c r="AV24" s="137"/>
-      <c r="AW24" s="136"/>
-      <c r="AX24" s="131"/>
-      <c r="AY24" s="131"/>
-      <c r="AZ24" s="131"/>
-      <c r="BA24" s="131"/>
-      <c r="BB24" s="131"/>
-      <c r="BC24" s="131"/>
-      <c r="BD24" s="131"/>
-      <c r="BE24" s="131"/>
-      <c r="BF24" s="131"/>
+      <c r="C24" s="126"/>
+      <c r="D24" s="127"/>
+      <c r="E24" s="127"/>
+      <c r="F24" s="127"/>
+      <c r="G24" s="127"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="127"/>
+      <c r="J24" s="127"/>
+      <c r="K24" s="127"/>
+      <c r="L24" s="127"/>
+      <c r="M24" s="127"/>
+      <c r="N24" s="128"/>
+      <c r="O24" s="126"/>
+      <c r="P24" s="127"/>
+      <c r="Q24" s="127"/>
+      <c r="R24" s="127"/>
+      <c r="S24" s="127"/>
+      <c r="T24" s="128"/>
+      <c r="U24" s="122"/>
+      <c r="V24" s="123"/>
+      <c r="W24" s="122"/>
+      <c r="X24" s="123"/>
+      <c r="Y24" s="122"/>
+      <c r="Z24" s="123"/>
+      <c r="AA24" s="122"/>
+      <c r="AB24" s="123"/>
+      <c r="AC24" s="122"/>
+      <c r="AD24" s="123"/>
+      <c r="AE24" s="122"/>
+      <c r="AF24" s="123"/>
+      <c r="AG24" s="122"/>
+      <c r="AH24" s="123"/>
+      <c r="AI24" s="122"/>
+      <c r="AJ24" s="123"/>
+      <c r="AK24" s="122"/>
+      <c r="AL24" s="123"/>
+      <c r="AM24" s="122"/>
+      <c r="AN24" s="124"/>
+      <c r="AO24" s="124"/>
+      <c r="AP24" s="124"/>
+      <c r="AQ24" s="124"/>
+      <c r="AR24" s="124"/>
+      <c r="AS24" s="124"/>
+      <c r="AT24" s="124"/>
+      <c r="AU24" s="124"/>
+      <c r="AV24" s="124"/>
+      <c r="AW24" s="123"/>
+      <c r="AX24" s="125"/>
+      <c r="AY24" s="125"/>
+      <c r="AZ24" s="125"/>
+      <c r="BA24" s="125"/>
+      <c r="BB24" s="125"/>
+      <c r="BC24" s="125"/>
+      <c r="BD24" s="125"/>
+      <c r="BE24" s="125"/>
+      <c r="BF24" s="125"/>
     </row>
   </sheetData>
   <mergeCells count="210">
-    <mergeCell ref="AE24:AF24"/>
-    <mergeCell ref="AG24:AH24"/>
-    <mergeCell ref="AI24:AJ24"/>
-    <mergeCell ref="AK24:AL24"/>
-    <mergeCell ref="AM24:AW24"/>
-    <mergeCell ref="AI23:AJ23"/>
-    <mergeCell ref="AK23:AL23"/>
-    <mergeCell ref="AM23:AW23"/>
-    <mergeCell ref="AX23:BF23"/>
+    <mergeCell ref="O8:T9"/>
+    <mergeCell ref="U8:V9"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="Y8:Z9"/>
+    <mergeCell ref="C8:N9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="AM8:AW9"/>
+    <mergeCell ref="AX8:BF9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AG9:AH9"/>
+    <mergeCell ref="AI9:AJ9"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AA8:AL8"/>
+    <mergeCell ref="AX10:BF10"/>
+    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="O11:T11"/>
+    <mergeCell ref="U11:V11"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="AE11:AF11"/>
+    <mergeCell ref="AG11:AH11"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="AE10:AF10"/>
+    <mergeCell ref="AG10:AH10"/>
+    <mergeCell ref="AI10:AJ10"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AM10:AW10"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AI11:AJ11"/>
+    <mergeCell ref="AK11:AL11"/>
+    <mergeCell ref="AM11:AW11"/>
+    <mergeCell ref="AX11:BF11"/>
+    <mergeCell ref="C12:N12"/>
+    <mergeCell ref="O12:T12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AX12:BF12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AE12:AF12"/>
+    <mergeCell ref="AG12:AH12"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AM12:AW12"/>
+    <mergeCell ref="AX13:BF13"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="O14:T14"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AX14:BF14"/>
+    <mergeCell ref="AC14:AD14"/>
+    <mergeCell ref="AE14:AF14"/>
+    <mergeCell ref="AG14:AH14"/>
+    <mergeCell ref="AI14:AJ14"/>
+    <mergeCell ref="AK14:AL14"/>
+    <mergeCell ref="AM14:AW14"/>
+    <mergeCell ref="C13:N13"/>
+    <mergeCell ref="O13:T13"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="AE13:AF13"/>
+    <mergeCell ref="AG13:AH13"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AG15:AH15"/>
+    <mergeCell ref="AI13:AJ13"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="AM13:AW13"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AC17:AD17"/>
+    <mergeCell ref="AE17:AF17"/>
+    <mergeCell ref="AG17:AH17"/>
+    <mergeCell ref="AI15:AJ15"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AM15:AW15"/>
+    <mergeCell ref="AX15:BF15"/>
+    <mergeCell ref="C16:N16"/>
+    <mergeCell ref="O16:T16"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="AX16:BF16"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="AE16:AF16"/>
+    <mergeCell ref="AG16:AH16"/>
+    <mergeCell ref="AI16:AJ16"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AM16:AW16"/>
+    <mergeCell ref="C15:N15"/>
+    <mergeCell ref="O15:T15"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="AE19:AF19"/>
+    <mergeCell ref="AG19:AH19"/>
+    <mergeCell ref="AI17:AJ17"/>
+    <mergeCell ref="AK17:AL17"/>
+    <mergeCell ref="AM17:AW17"/>
+    <mergeCell ref="AX17:BF17"/>
+    <mergeCell ref="C18:N18"/>
+    <mergeCell ref="O18:T18"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="AA18:AB18"/>
+    <mergeCell ref="AX18:BF18"/>
+    <mergeCell ref="AC18:AD18"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="AG18:AH18"/>
+    <mergeCell ref="AI18:AJ18"/>
+    <mergeCell ref="AK18:AL18"/>
+    <mergeCell ref="AM18:AW18"/>
+    <mergeCell ref="C17:N17"/>
+    <mergeCell ref="O17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="AI19:AJ19"/>
+    <mergeCell ref="AK19:AL19"/>
+    <mergeCell ref="AM19:AW19"/>
+    <mergeCell ref="AX19:BF19"/>
+    <mergeCell ref="C20:N20"/>
+    <mergeCell ref="O20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AX20:BF20"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="AE20:AF20"/>
+    <mergeCell ref="AG20:AH20"/>
+    <mergeCell ref="AI20:AJ20"/>
+    <mergeCell ref="AK20:AL20"/>
+    <mergeCell ref="AM20:AW20"/>
+    <mergeCell ref="C19:N19"/>
+    <mergeCell ref="O19:T19"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="AC19:AD19"/>
+    <mergeCell ref="AI21:AJ21"/>
+    <mergeCell ref="AK21:AL21"/>
+    <mergeCell ref="AM21:AW21"/>
+    <mergeCell ref="AX21:BF21"/>
+    <mergeCell ref="C22:N22"/>
+    <mergeCell ref="O22:T22"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="C21:N21"/>
+    <mergeCell ref="O21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="AE21:AF21"/>
+    <mergeCell ref="AG21:AH21"/>
     <mergeCell ref="C24:N24"/>
     <mergeCell ref="O24:T24"/>
     <mergeCell ref="U24:V24"/>
@@ -26525,183 +26687,15 @@
     <mergeCell ref="AM22:AW22"/>
     <mergeCell ref="AX24:BF24"/>
     <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="AI21:AJ21"/>
-    <mergeCell ref="AK21:AL21"/>
-    <mergeCell ref="AM21:AW21"/>
-    <mergeCell ref="AX21:BF21"/>
-    <mergeCell ref="C22:N22"/>
-    <mergeCell ref="O22:T22"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="C21:N21"/>
-    <mergeCell ref="O21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="AE21:AF21"/>
-    <mergeCell ref="AG21:AH21"/>
-    <mergeCell ref="AI19:AJ19"/>
-    <mergeCell ref="AK19:AL19"/>
-    <mergeCell ref="AM19:AW19"/>
-    <mergeCell ref="AX19:BF19"/>
-    <mergeCell ref="C20:N20"/>
-    <mergeCell ref="O20:T20"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AX20:BF20"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="AE20:AF20"/>
-    <mergeCell ref="AG20:AH20"/>
-    <mergeCell ref="AI20:AJ20"/>
-    <mergeCell ref="AK20:AL20"/>
-    <mergeCell ref="AM20:AW20"/>
-    <mergeCell ref="C19:N19"/>
-    <mergeCell ref="O19:T19"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="W19:X19"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="AA19:AB19"/>
-    <mergeCell ref="AC19:AD19"/>
-    <mergeCell ref="AE19:AF19"/>
-    <mergeCell ref="AG19:AH19"/>
-    <mergeCell ref="AI17:AJ17"/>
-    <mergeCell ref="AK17:AL17"/>
-    <mergeCell ref="AM17:AW17"/>
-    <mergeCell ref="AX17:BF17"/>
-    <mergeCell ref="C18:N18"/>
-    <mergeCell ref="O18:T18"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="W18:X18"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="AA18:AB18"/>
-    <mergeCell ref="AX18:BF18"/>
-    <mergeCell ref="AC18:AD18"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="AG18:AH18"/>
-    <mergeCell ref="AI18:AJ18"/>
-    <mergeCell ref="AK18:AL18"/>
-    <mergeCell ref="AM18:AW18"/>
-    <mergeCell ref="C17:N17"/>
-    <mergeCell ref="O17:T17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="AC17:AD17"/>
-    <mergeCell ref="AE17:AF17"/>
-    <mergeCell ref="AG17:AH17"/>
-    <mergeCell ref="AI15:AJ15"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AM15:AW15"/>
-    <mergeCell ref="AX15:BF15"/>
-    <mergeCell ref="C16:N16"/>
-    <mergeCell ref="O16:T16"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AX16:BF16"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="AE16:AF16"/>
-    <mergeCell ref="AG16:AH16"/>
-    <mergeCell ref="AI16:AJ16"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AM16:AW16"/>
-    <mergeCell ref="C15:N15"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="AG15:AH15"/>
-    <mergeCell ref="AI13:AJ13"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="AM13:AW13"/>
-    <mergeCell ref="AX13:BF13"/>
-    <mergeCell ref="C14:N14"/>
-    <mergeCell ref="O14:T14"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AX14:BF14"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="AE14:AF14"/>
-    <mergeCell ref="AG14:AH14"/>
-    <mergeCell ref="AI14:AJ14"/>
-    <mergeCell ref="AK14:AL14"/>
-    <mergeCell ref="AM14:AW14"/>
-    <mergeCell ref="C13:N13"/>
-    <mergeCell ref="O13:T13"/>
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="AE13:AF13"/>
-    <mergeCell ref="AG13:AH13"/>
-    <mergeCell ref="AM11:AW11"/>
-    <mergeCell ref="AX11:BF11"/>
-    <mergeCell ref="C12:N12"/>
-    <mergeCell ref="O12:T12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AX12:BF12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="AE12:AF12"/>
-    <mergeCell ref="AG12:AH12"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AM12:AW12"/>
-    <mergeCell ref="AX10:BF10"/>
-    <mergeCell ref="C11:N11"/>
-    <mergeCell ref="O11:T11"/>
-    <mergeCell ref="U11:V11"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="AE11:AF11"/>
-    <mergeCell ref="AG11:AH11"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="AE10:AF10"/>
-    <mergeCell ref="AG10:AH10"/>
-    <mergeCell ref="AI10:AJ10"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AM10:AW10"/>
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AI11:AJ11"/>
-    <mergeCell ref="AK11:AL11"/>
-    <mergeCell ref="O8:T9"/>
-    <mergeCell ref="U8:V9"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="Y8:Z9"/>
-    <mergeCell ref="C8:N9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="AM8:AW9"/>
-    <mergeCell ref="AX8:BF9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="AE9:AF9"/>
-    <mergeCell ref="AG9:AH9"/>
-    <mergeCell ref="AI9:AJ9"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="AA8:AL8"/>
+    <mergeCell ref="AE24:AF24"/>
+    <mergeCell ref="AG24:AH24"/>
+    <mergeCell ref="AI24:AJ24"/>
+    <mergeCell ref="AK24:AL24"/>
+    <mergeCell ref="AM24:AW24"/>
+    <mergeCell ref="AI23:AJ23"/>
+    <mergeCell ref="AK23:AL23"/>
+    <mergeCell ref="AM23:AW23"/>
+    <mergeCell ref="AX23:BF23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26718,7 +26712,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AY5" sqref="AY5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -26784,7 +26780,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -26800,7 +26796,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>
@@ -28562,7 +28558,7 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="10"/>
       <c r="AM4" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="AN4" s="13"/>
       <c r="AO4" s="13"/>
@@ -28578,7 +28574,7 @@
       <c r="AW4" s="9"/>
       <c r="AX4" s="10"/>
       <c r="AY4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AZ4" s="13"/>
       <c r="BA4" s="13"/>

</xml_diff>